<commit_message>
DRI global settings to use either increment or total specification
</commit_message>
<xml_diff>
--- a/Input/controlTotals/FLUAM_DRI.xlsx
+++ b/Input/controlTotals/FLUAM_DRI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Models\StateWide\TSM_Legacy\FLUAM\Input\controlTotals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A000017-D057-48EC-A06A-ED6B138579A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372F1889-27D9-40DE-82CE-7562583E04C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4793C3-9AA2-4A53-B6D8-945A8B7F0D49}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4793C3-9AA2-4A53-B6D8-945A8B7F0D49}"/>
   </bookViews>
   <sheets>
     <sheet name="DRIs" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t xml:space="preserve"> employment</t>
   </si>
   <si>
-    <t>2015.Parcel.HH</t>
-  </si>
-  <si>
     <t>2015.Parcel_EMP</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Instead supply the same controls at TAZ level and let user decide how FLUAM should allocate</t>
+  </si>
+  <si>
+    <t>2015.Parcel_HH</t>
   </si>
 </sst>
 </file>
@@ -522,10 +522,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -825,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44179D55-CFD5-47AC-81DE-5AB054DCBB5F}">
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,10 +850,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>0</v>
@@ -5831,7 +5827,7 @@
   <dimension ref="A1:Q99"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12517,7 +12513,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -12556,27 +12552,27 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vacant land for development = available + developed (required to allow MPO specified aggregate numbers).
</commit_message>
<xml_diff>
--- a/Input/controlTotals/FLUAM_DRI.xlsx
+++ b/Input/controlTotals/FLUAM_DRI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Models\StateWide\TSM_Legacy\FLUAM\Input\controlTotals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372F1889-27D9-40DE-82CE-7562583E04C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E647C-67B2-4528-920F-1BBBF97F358B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4793C3-9AA2-4A53-B6D8-945A8B7F0D49}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0A4793C3-9AA2-4A53-B6D8-945A8B7F0D49}"/>
   </bookViews>
   <sheets>
     <sheet name="DRIs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>2020.DRI_HH</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>2015.Parcel_HH</t>
+  </si>
+  <si>
+    <t>Total35y.DRI_HH</t>
+  </si>
+  <si>
+    <t>Total35y.DRI_EMP</t>
   </si>
 </sst>
 </file>
@@ -430,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -504,6 +510,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -821,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44179D55-CFD5-47AC-81DE-5AB054DCBB5F}">
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S1" sqref="R1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5824,10 +5831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56B04E6-F45C-49E4-A13B-3B72B1122121}">
-  <dimension ref="A1:Q99"/>
+  <dimension ref="A1:S99"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5839,12 +5846,13 @@
     <col min="12" max="12" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="9.140625" style="3"/>
     <col min="17" max="17" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.85546875"/>
     <col min="24" max="24" width="8.85546875"/>
     <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>14</v>
       </c>
@@ -5896,8 +5904,14 @@
       <c r="Q1" s="25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R1" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>32</v>
       </c>
@@ -5963,8 +5977,16 @@
         <f>DRIs!Q2-DRIs!O2</f>
         <v>1575</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R2" s="3">
+        <f>D2+F2+H2+J2+L2+N2+P2</f>
+        <v>9961</v>
+      </c>
+      <c r="S2" s="3">
+        <f>E2+G2+I2+K2+M2+O2+Q2</f>
+        <v>6980</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>48</v>
       </c>
@@ -6030,8 +6052,16 @@
         <f>DRIs!Q3-DRIs!O3</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R3" s="3">
+        <f t="shared" ref="R3:R66" si="0">D3+F3+H3+J3+L3+N3+P3</f>
+        <v>224</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S66" si="1">E3+G3+I3+K3+M3+O3+Q3</f>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>51</v>
       </c>
@@ -6097,8 +6127,16 @@
         <f>DRIs!Q4-DRIs!O4</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R4" s="3">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>58</v>
       </c>
@@ -6164,8 +6202,16 @@
         <f>DRIs!Q5-DRIs!O5</f>
         <v>141</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R5" s="3">
+        <f t="shared" si="0"/>
+        <v>620</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="1"/>
+        <v>653</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>72</v>
       </c>
@@ -6231,8 +6277,16 @@
         <f>DRIs!Q6-DRIs!O6</f>
         <v>360</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R6" s="3">
+        <f t="shared" si="0"/>
+        <v>4264</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" si="1"/>
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>84</v>
       </c>
@@ -6298,8 +6352,16 @@
         <f>DRIs!Q7-DRIs!O7</f>
         <v>210</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R7" s="3">
+        <f t="shared" si="0"/>
+        <v>2291</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="1"/>
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>133</v>
       </c>
@@ -6365,8 +6427,16 @@
         <f>DRIs!Q8-DRIs!O8</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R8" s="3">
+        <f t="shared" si="0"/>
+        <v>1427</v>
+      </c>
+      <c r="S8" s="3">
+        <f t="shared" si="1"/>
+        <v>814</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>163</v>
       </c>
@@ -6432,8 +6502,16 @@
         <f>DRIs!Q9-DRIs!O9</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R9" s="3">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+      <c r="S9" s="3">
+        <f t="shared" si="1"/>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>206</v>
       </c>
@@ -6499,8 +6577,16 @@
         <f>DRIs!Q10-DRIs!O10</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R10" s="3">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="S10" s="3">
+        <f t="shared" si="1"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>208</v>
       </c>
@@ -6566,8 +6652,16 @@
         <f>DRIs!Q11-DRIs!O11</f>
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R11" s="3">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="S11" s="3">
+        <f t="shared" si="1"/>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>287</v>
       </c>
@@ -6633,8 +6727,16 @@
         <f>DRIs!Q12-DRIs!O12</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R12" s="3">
+        <f t="shared" si="0"/>
+        <v>817</v>
+      </c>
+      <c r="S12" s="3">
+        <f t="shared" si="1"/>
+        <v>948</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>309</v>
       </c>
@@ -6700,8 +6802,16 @@
         <f>DRIs!Q13-DRIs!O13</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R13" s="3">
+        <f t="shared" si="0"/>
+        <v>756</v>
+      </c>
+      <c r="S13" s="3">
+        <f t="shared" si="1"/>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>369</v>
       </c>
@@ -6767,8 +6877,16 @@
         <f>DRIs!Q14-DRIs!O14</f>
         <v>135</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R14" s="3">
+        <f t="shared" si="0"/>
+        <v>1789</v>
+      </c>
+      <c r="S14" s="3">
+        <f t="shared" si="1"/>
+        <v>852</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>371</v>
       </c>
@@ -6834,8 +6952,16 @@
         <f>DRIs!Q15-DRIs!O15</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R15" s="3">
+        <f t="shared" si="0"/>
+        <v>1410</v>
+      </c>
+      <c r="S15" s="3">
+        <f t="shared" si="1"/>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>431</v>
       </c>
@@ -6901,8 +7027,16 @@
         <f>DRIs!Q16-DRIs!O16</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R16" s="3">
+        <f t="shared" si="0"/>
+        <v>1312</v>
+      </c>
+      <c r="S16" s="3">
+        <f t="shared" si="1"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>470</v>
       </c>
@@ -6968,8 +7102,16 @@
         <f>DRIs!Q17-DRIs!O17</f>
         <v>570</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R17" s="3">
+        <f t="shared" si="0"/>
+        <v>3254</v>
+      </c>
+      <c r="S17" s="3">
+        <f t="shared" si="1"/>
+        <v>3436</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>513</v>
       </c>
@@ -7035,8 +7177,16 @@
         <f>DRIs!Q18-DRIs!O18</f>
         <v>141</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R18" s="3">
+        <f t="shared" si="0"/>
+        <v>5546</v>
+      </c>
+      <c r="S18" s="3">
+        <f t="shared" si="1"/>
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>516</v>
       </c>
@@ -7102,8 +7252,16 @@
         <f>DRIs!Q19-DRIs!O19</f>
         <v>222</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R19" s="3">
+        <f t="shared" si="0"/>
+        <v>2193</v>
+      </c>
+      <c r="S19" s="3">
+        <f t="shared" si="1"/>
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>520</v>
       </c>
@@ -7169,8 +7327,16 @@
         <f>DRIs!Q20-DRIs!O20</f>
         <v>1050</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R20" s="3">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+      <c r="S20" s="3">
+        <f t="shared" si="1"/>
+        <v>4662</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>621</v>
       </c>
@@ -7236,8 +7402,16 @@
         <f>DRIs!Q21-DRIs!O21</f>
         <v>390</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R21" s="3">
+        <f t="shared" si="0"/>
+        <v>194</v>
+      </c>
+      <c r="S21" s="3">
+        <f t="shared" si="1"/>
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>625</v>
       </c>
@@ -7303,8 +7477,16 @@
         <f>DRIs!Q22-DRIs!O22</f>
         <v>435</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R22" s="3">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="S22" s="3">
+        <f t="shared" si="1"/>
+        <v>2551</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>695</v>
       </c>
@@ -7370,8 +7552,16 @@
         <f>DRIs!Q23-DRIs!O23</f>
         <v>264</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R23" s="3">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="S23" s="3">
+        <f t="shared" si="1"/>
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <v>700</v>
       </c>
@@ -7437,8 +7627,16 @@
         <f>DRIs!Q24-DRIs!O24</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R24" s="3">
+        <f t="shared" si="0"/>
+        <v>1108</v>
+      </c>
+      <c r="S24" s="3">
+        <f t="shared" si="1"/>
+        <v>879</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
         <v>702</v>
       </c>
@@ -7504,8 +7702,16 @@
         <f>DRIs!Q25-DRIs!O25</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R25" s="3">
+        <f t="shared" si="0"/>
+        <v>199</v>
+      </c>
+      <c r="S25" s="3">
+        <f t="shared" si="1"/>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>703</v>
       </c>
@@ -7571,8 +7777,16 @@
         <f>DRIs!Q26-DRIs!O26</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R26" s="3">
+        <f t="shared" si="0"/>
+        <v>191</v>
+      </c>
+      <c r="S26" s="3">
+        <f t="shared" si="1"/>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>716</v>
       </c>
@@ -7638,8 +7852,16 @@
         <f>DRIs!Q27-DRIs!O27</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R27" s="3">
+        <f t="shared" si="0"/>
+        <v>925</v>
+      </c>
+      <c r="S27" s="3">
+        <f t="shared" si="1"/>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>718</v>
       </c>
@@ -7705,8 +7927,16 @@
         <f>DRIs!Q28-DRIs!O28</f>
         <v>955</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R28" s="3">
+        <f t="shared" si="0"/>
+        <v>10617</v>
+      </c>
+      <c r="S28" s="3">
+        <f t="shared" si="1"/>
+        <v>6350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>721</v>
       </c>
@@ -7772,8 +8002,16 @@
         <f>DRIs!Q29-DRIs!O29</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R29" s="3">
+        <f t="shared" si="0"/>
+        <v>704</v>
+      </c>
+      <c r="S29" s="3">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>810</v>
       </c>
@@ -7839,8 +8077,16 @@
         <f>DRIs!Q30-DRIs!O30</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R30" s="3">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="S30" s="3">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>811</v>
       </c>
@@ -7906,8 +8152,16 @@
         <f>DRIs!Q31-DRIs!O31</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R31" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="S31" s="3">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>812</v>
       </c>
@@ -7973,8 +8227,16 @@
         <f>DRIs!Q32-DRIs!O32</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R32" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="S32" s="3">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>1515</v>
       </c>
@@ -8040,8 +8302,16 @@
         <f>DRIs!Q33-DRIs!O33</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R33" s="3">
+        <f t="shared" si="0"/>
+        <v>328</v>
+      </c>
+      <c r="S33" s="3">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16">
         <v>1725</v>
       </c>
@@ -8107,8 +8377,16 @@
         <f>DRIs!Q34-DRIs!O34</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R34" s="3">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="S34" s="3">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16">
         <v>1728</v>
       </c>
@@ -8174,8 +8452,16 @@
         <f>DRIs!Q35-DRIs!O35</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R35" s="3">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+      <c r="S35" s="3">
+        <f t="shared" si="1"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>1733</v>
       </c>
@@ -8241,8 +8527,16 @@
         <f>DRIs!Q36-DRIs!O36</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R36" s="3">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="S36" s="3">
+        <f t="shared" si="1"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>3520</v>
       </c>
@@ -8308,8 +8602,16 @@
         <f>DRIs!Q37-DRIs!O37</f>
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R37" s="3">
+        <f t="shared" si="0"/>
+        <v>2143</v>
+      </c>
+      <c r="S37" s="3">
+        <f t="shared" si="1"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <v>3522</v>
       </c>
@@ -8375,8 +8677,16 @@
         <f>DRIs!Q38-DRIs!O38</f>
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R38" s="3">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="S38" s="3">
+        <f t="shared" si="1"/>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <v>3527</v>
       </c>
@@ -8442,8 +8752,16 @@
         <f>DRIs!Q39-DRIs!O39</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R39" s="3">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="S39" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16">
         <v>3534</v>
       </c>
@@ -8509,8 +8827,16 @@
         <f>DRIs!Q40-DRIs!O40</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R40" s="3">
+        <f t="shared" si="0"/>
+        <v>2705</v>
+      </c>
+      <c r="S40" s="3">
+        <f t="shared" si="1"/>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>3569</v>
       </c>
@@ -8576,8 +8902,16 @@
         <f>DRIs!Q41-DRIs!O41</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R41" s="3">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="S41" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16">
         <v>3577</v>
       </c>
@@ -8643,8 +8977,16 @@
         <f>DRIs!Q42-DRIs!O42</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R42" s="3">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="S42" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16">
         <v>3578</v>
       </c>
@@ -8710,8 +9052,16 @@
         <f>DRIs!Q43-DRIs!O43</f>
         <v>79</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R43" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S43" s="3">
+        <f t="shared" si="1"/>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16">
         <v>3580</v>
       </c>
@@ -8777,8 +9127,16 @@
         <f>DRIs!Q44-DRIs!O44</f>
         <v>225</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R44" s="3">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="S44" s="3">
+        <f t="shared" si="1"/>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16">
         <v>3581</v>
       </c>
@@ -8844,8 +9202,16 @@
         <f>DRIs!Q45-DRIs!O45</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R45" s="3">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="S45" s="3">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16">
         <v>3582</v>
       </c>
@@ -8911,8 +9277,16 @@
         <f>DRIs!Q46-DRIs!O46</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R46" s="3">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S46" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="17">
         <v>3583</v>
       </c>
@@ -8978,8 +9352,16 @@
         <f>DRIs!Q47-DRIs!O47</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R47" s="3">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="S47" s="3">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17">
         <v>3590</v>
       </c>
@@ -9045,8 +9427,16 @@
         <f>DRIs!Q48-DRIs!O48</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R48" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S48" s="3">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="17">
         <v>3593</v>
       </c>
@@ -9112,8 +9502,16 @@
         <f>DRIs!Q49-DRIs!O49</f>
         <v>142</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R49" s="3">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="S49" s="3">
+        <f t="shared" si="1"/>
+        <v>475</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="17">
         <v>3595</v>
       </c>
@@ -9179,8 +9577,16 @@
         <f>DRIs!Q50-DRIs!O50</f>
         <v>112</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R50" s="3">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="S50" s="3">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="17">
         <v>3600</v>
       </c>
@@ -9246,8 +9652,16 @@
         <f>DRIs!Q51-DRIs!O51</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R51" s="3">
+        <f t="shared" si="0"/>
+        <v>675</v>
+      </c>
+      <c r="S51" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="17">
         <v>3602</v>
       </c>
@@ -9313,8 +9727,16 @@
         <f>DRIs!Q52-DRIs!O52</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R52" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S52" s="3">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17">
         <v>3610</v>
       </c>
@@ -9380,8 +9802,16 @@
         <f>DRIs!Q53-DRIs!O53</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R53" s="3">
+        <f t="shared" si="0"/>
+        <v>525</v>
+      </c>
+      <c r="S53" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="17">
         <v>3611</v>
       </c>
@@ -9447,8 +9877,16 @@
         <f>DRIs!Q54-DRIs!O54</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R54" s="3">
+        <f t="shared" si="0"/>
+        <v>1095</v>
+      </c>
+      <c r="S54" s="3">
+        <f t="shared" si="1"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17">
         <v>3612</v>
       </c>
@@ -9514,8 +9952,16 @@
         <f>DRIs!Q55-DRIs!O55</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R55" s="3">
+        <f t="shared" si="0"/>
+        <v>2440</v>
+      </c>
+      <c r="S55" s="3">
+        <f t="shared" si="1"/>
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17">
         <v>3613</v>
       </c>
@@ -9581,8 +10027,16 @@
         <f>DRIs!Q56-DRIs!O56</f>
         <v>975</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R56" s="3">
+        <f t="shared" si="0"/>
+        <v>5789</v>
+      </c>
+      <c r="S56" s="3">
+        <f t="shared" si="1"/>
+        <v>5953</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17">
         <v>3614</v>
       </c>
@@ -9648,8 +10102,16 @@
         <f>DRIs!Q57-DRIs!O57</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R57" s="3">
+        <f t="shared" si="0"/>
+        <v>202</v>
+      </c>
+      <c r="S57" s="3">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="17">
         <v>3616</v>
       </c>
@@ -9715,8 +10177,16 @@
         <f>DRIs!Q58-DRIs!O58</f>
         <v>165</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R58" s="3">
+        <f t="shared" si="0"/>
+        <v>3848</v>
+      </c>
+      <c r="S58" s="3">
+        <f t="shared" si="1"/>
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="17">
         <v>3617</v>
       </c>
@@ -9782,8 +10252,16 @@
         <f>DRIs!Q59-DRIs!O59</f>
         <v>285</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R59" s="3">
+        <f t="shared" si="0"/>
+        <v>698</v>
+      </c>
+      <c r="S59" s="3">
+        <f t="shared" si="1"/>
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="17">
         <v>3709</v>
       </c>
@@ -9849,8 +10327,16 @@
         <f>DRIs!Q60-DRIs!O60</f>
         <v>270</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R60" s="3">
+        <f t="shared" si="0"/>
+        <v>1309</v>
+      </c>
+      <c r="S60" s="3">
+        <f t="shared" si="1"/>
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="17">
         <v>3739</v>
       </c>
@@ -9916,8 +10402,16 @@
         <f>DRIs!Q61-DRIs!O61</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R61" s="3">
+        <f t="shared" si="0"/>
+        <v>1093</v>
+      </c>
+      <c r="S61" s="3">
+        <f t="shared" si="1"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="17">
         <v>3772</v>
       </c>
@@ -9983,8 +10477,16 @@
         <f>DRIs!Q62-DRIs!O62</f>
         <v>450</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R62" s="3">
+        <f t="shared" si="0"/>
+        <v>3438</v>
+      </c>
+      <c r="S62" s="3">
+        <f t="shared" si="1"/>
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="17">
         <v>3793</v>
       </c>
@@ -10050,8 +10552,16 @@
         <f>DRIs!Q63-DRIs!O63</f>
         <v>303</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R63" s="3">
+        <f t="shared" si="0"/>
+        <v>645</v>
+      </c>
+      <c r="S63" s="3">
+        <f t="shared" si="1"/>
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="17">
         <v>3806</v>
       </c>
@@ -10117,8 +10627,16 @@
         <f>DRIs!Q64-DRIs!O64</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R64" s="3">
+        <f t="shared" si="0"/>
+        <v>780</v>
+      </c>
+      <c r="S64" s="3">
+        <f t="shared" si="1"/>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="17">
         <v>3822</v>
       </c>
@@ -10184,8 +10702,16 @@
         <f>DRIs!Q65-DRIs!O65</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R65" s="3">
+        <f t="shared" si="0"/>
+        <v>615</v>
+      </c>
+      <c r="S65" s="3">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17">
         <v>3823</v>
       </c>
@@ -10251,8 +10777,16 @@
         <f>DRIs!Q66-DRIs!O66</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R66" s="3">
+        <f t="shared" si="0"/>
+        <v>425</v>
+      </c>
+      <c r="S66" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="17">
         <v>3834</v>
       </c>
@@ -10318,8 +10852,16 @@
         <f>DRIs!Q67-DRIs!O67</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R67" s="3">
+        <f t="shared" ref="R67:R99" si="2">D67+F67+H67+J67+L67+N67+P67</f>
+        <v>350</v>
+      </c>
+      <c r="S67" s="3">
+        <f t="shared" ref="S67:S99" si="3">E67+G67+I67+K67+M67+O67+Q67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="17">
         <v>3835</v>
       </c>
@@ -10385,8 +10927,16 @@
         <f>DRIs!Q68-DRIs!O68</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R68" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S68" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="17">
         <v>3848</v>
       </c>
@@ -10452,8 +11002,16 @@
         <f>DRIs!Q69-DRIs!O69</f>
         <v>180</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R69" s="3">
+        <f t="shared" si="2"/>
+        <v>1100</v>
+      </c>
+      <c r="S69" s="3">
+        <f t="shared" si="3"/>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="17">
         <v>3852</v>
       </c>
@@ -10519,8 +11077,16 @@
         <f>DRIs!Q70-DRIs!O70</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R70" s="3">
+        <f t="shared" si="2"/>
+        <v>3505</v>
+      </c>
+      <c r="S70" s="3">
+        <f t="shared" si="3"/>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="17">
         <v>3859</v>
       </c>
@@ -10586,8 +11152,16 @@
         <f>DRIs!Q71-DRIs!O71</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R71" s="3">
+        <f t="shared" si="2"/>
+        <v>692</v>
+      </c>
+      <c r="S71" s="3">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="17">
         <v>3871</v>
       </c>
@@ -10653,8 +11227,16 @@
         <f>DRIs!Q72-DRIs!O72</f>
         <v>156</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R72" s="3">
+        <f t="shared" si="2"/>
+        <v>4809</v>
+      </c>
+      <c r="S72" s="3">
+        <f t="shared" si="3"/>
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="17">
         <v>4124</v>
       </c>
@@ -10720,8 +11302,16 @@
         <f>DRIs!Q73-DRIs!O73</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R73" s="3">
+        <f t="shared" si="2"/>
+        <v>11003</v>
+      </c>
+      <c r="S73" s="3">
+        <f t="shared" si="3"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>4125</v>
       </c>
@@ -10787,8 +11377,16 @@
         <f>DRIs!Q74-DRIs!O74</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R74" s="3">
+        <f t="shared" si="2"/>
+        <v>3370</v>
+      </c>
+      <c r="S74" s="3">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="17">
         <v>4126</v>
       </c>
@@ -10854,8 +11452,16 @@
         <f>DRIs!Q75-DRIs!O75</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R75" s="3">
+        <f t="shared" si="2"/>
+        <v>1194</v>
+      </c>
+      <c r="S75" s="3">
+        <f t="shared" si="3"/>
+        <v>487</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="17">
         <v>4165</v>
       </c>
@@ -10921,8 +11527,16 @@
         <f>DRIs!Q76-DRIs!O76</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R76" s="3">
+        <f t="shared" si="2"/>
+        <v>2500</v>
+      </c>
+      <c r="S76" s="3">
+        <f t="shared" si="3"/>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="17">
         <v>4166</v>
       </c>
@@ -10988,8 +11602,16 @@
         <f>DRIs!Q77-DRIs!O77</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R77" s="3">
+        <f t="shared" si="2"/>
+        <v>1750</v>
+      </c>
+      <c r="S77" s="3">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="17">
         <v>4186</v>
       </c>
@@ -11055,8 +11677,16 @@
         <f>DRIs!Q78-DRIs!O78</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R78" s="3">
+        <f t="shared" si="2"/>
+        <v>3996</v>
+      </c>
+      <c r="S78" s="3">
+        <f t="shared" si="3"/>
+        <v>783</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="17">
         <v>4189</v>
       </c>
@@ -11122,8 +11752,16 @@
         <f>DRIs!Q79-DRIs!O79</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R79" s="3">
+        <f t="shared" si="2"/>
+        <v>650</v>
+      </c>
+      <c r="S79" s="3">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="17">
         <v>4190</v>
       </c>
@@ -11189,8 +11827,16 @@
         <f>DRIs!Q80-DRIs!O80</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R80" s="3">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="S80" s="3">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="17">
         <v>4236</v>
       </c>
@@ -11256,8 +11902,16 @@
         <f>DRIs!Q81-DRIs!O81</f>
         <v>318</v>
       </c>
-    </row>
-    <row r="82" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R81" s="3">
+        <f t="shared" si="2"/>
+        <v>2291</v>
+      </c>
+      <c r="S81" s="3">
+        <f t="shared" si="3"/>
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="17">
         <v>4264</v>
       </c>
@@ -11323,8 +11977,16 @@
         <f>DRIs!Q82-DRIs!O82</f>
         <v>810</v>
       </c>
-    </row>
-    <row r="83" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R82" s="3">
+        <f t="shared" si="2"/>
+        <v>7469</v>
+      </c>
+      <c r="S82" s="3">
+        <f t="shared" si="3"/>
+        <v>5383</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="17">
         <v>4267</v>
       </c>
@@ -11390,8 +12052,16 @@
         <f>DRIs!Q83-DRIs!O83</f>
         <v>144</v>
       </c>
-    </row>
-    <row r="84" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R83" s="3">
+        <f t="shared" si="2"/>
+        <v>5497</v>
+      </c>
+      <c r="S83" s="3">
+        <f t="shared" si="3"/>
+        <v>961</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="17">
         <v>4269</v>
       </c>
@@ -11457,8 +12127,16 @@
         <f>DRIs!Q84-DRIs!O84</f>
         <v>160</v>
       </c>
-    </row>
-    <row r="85" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R84" s="3">
+        <f t="shared" si="2"/>
+        <v>6502</v>
+      </c>
+      <c r="S84" s="3">
+        <f t="shared" si="3"/>
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="17">
         <v>4271</v>
       </c>
@@ -11524,8 +12202,16 @@
         <f>DRIs!Q85-DRIs!O85</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="86" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R85" s="3">
+        <f t="shared" si="2"/>
+        <v>2950</v>
+      </c>
+      <c r="S85" s="3">
+        <f t="shared" si="3"/>
+        <v>535</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="17">
         <v>4279</v>
       </c>
@@ -11591,8 +12277,16 @@
         <f>DRIs!Q86-DRIs!O86</f>
         <v>1800</v>
       </c>
-    </row>
-    <row r="87" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R86" s="3">
+        <f t="shared" si="2"/>
+        <v>1455</v>
+      </c>
+      <c r="S86" s="3">
+        <f t="shared" si="3"/>
+        <v>5008</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="17">
         <v>4508</v>
       </c>
@@ -11658,8 +12352,16 @@
         <f>DRIs!Q87-DRIs!O87</f>
         <v>79</v>
       </c>
-    </row>
-    <row r="88" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R87" s="3">
+        <f t="shared" si="2"/>
+        <v>4495</v>
+      </c>
+      <c r="S87" s="3">
+        <f t="shared" si="3"/>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="17">
         <v>4509</v>
       </c>
@@ -11725,8 +12427,16 @@
         <f>DRIs!Q88-DRIs!O88</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R88" s="3">
+        <f t="shared" si="2"/>
+        <v>2320</v>
+      </c>
+      <c r="S88" s="3">
+        <f t="shared" si="3"/>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="17">
         <v>4510</v>
       </c>
@@ -11792,8 +12502,16 @@
         <f>DRIs!Q89-DRIs!O89</f>
         <v>270</v>
       </c>
-    </row>
-    <row r="90" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R89" s="3">
+        <f t="shared" si="2"/>
+        <v>1481</v>
+      </c>
+      <c r="S89" s="3">
+        <f t="shared" si="3"/>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="17">
         <v>4532</v>
       </c>
@@ -11859,8 +12577,16 @@
         <f>DRIs!Q90-DRIs!O90</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="91" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R90" s="3">
+        <f t="shared" si="2"/>
+        <v>2750</v>
+      </c>
+      <c r="S90" s="3">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="17">
         <v>4534</v>
       </c>
@@ -11926,8 +12652,16 @@
         <f>DRIs!Q91-DRIs!O91</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="92" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R91" s="3">
+        <f t="shared" si="2"/>
+        <v>456</v>
+      </c>
+      <c r="S91" s="3">
+        <f t="shared" si="3"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="17">
         <v>4535</v>
       </c>
@@ -11993,8 +12727,16 @@
         <f>DRIs!Q92-DRIs!O92</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="93" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R92" s="3">
+        <f t="shared" si="2"/>
+        <v>1230</v>
+      </c>
+      <c r="S92" s="3">
+        <f t="shared" si="3"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="17">
         <v>4545</v>
       </c>
@@ -12060,8 +12802,16 @@
         <f>DRIs!Q93-DRIs!O93</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="94" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R93" s="3">
+        <f t="shared" si="2"/>
+        <v>2626</v>
+      </c>
+      <c r="S93" s="3">
+        <f t="shared" si="3"/>
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="17">
         <v>4753</v>
       </c>
@@ -12127,8 +12877,16 @@
         <f>DRIs!Q94-DRIs!O94</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="95" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R94" s="3">
+        <f t="shared" si="2"/>
+        <v>728</v>
+      </c>
+      <c r="S94" s="3">
+        <f t="shared" si="3"/>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="17">
         <v>4957</v>
       </c>
@@ -12194,8 +12952,16 @@
         <f>DRIs!Q95-DRIs!O95</f>
         <v>510</v>
       </c>
-    </row>
-    <row r="96" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R95" s="3">
+        <f t="shared" si="2"/>
+        <v>682</v>
+      </c>
+      <c r="S95" s="3">
+        <f t="shared" si="3"/>
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="17">
         <v>5280</v>
       </c>
@@ -12261,8 +13027,16 @@
         <f>DRIs!Q96-DRIs!O96</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="97" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R96" s="3">
+        <f t="shared" si="2"/>
+        <v>4345</v>
+      </c>
+      <c r="S96" s="3">
+        <f t="shared" si="3"/>
+        <v>889</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="17">
         <v>5283</v>
       </c>
@@ -12328,8 +13102,16 @@
         <f>DRIs!Q97-DRIs!O97</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="98" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R97" s="3">
+        <f t="shared" si="2"/>
+        <v>543</v>
+      </c>
+      <c r="S97" s="3">
+        <f t="shared" si="3"/>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="17">
         <v>5289</v>
       </c>
@@ -12395,8 +13177,16 @@
         <f>DRIs!Q98-DRIs!O98</f>
         <v>195</v>
       </c>
-    </row>
-    <row r="99" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R98" s="3">
+        <f t="shared" si="2"/>
+        <v>743</v>
+      </c>
+      <c r="S98" s="3">
+        <f t="shared" si="3"/>
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="18">
         <v>5294</v>
       </c>
@@ -12461,6 +13251,14 @@
       <c r="Q99" s="20">
         <f>DRIs!Q99-DRIs!O99</f>
         <v>60</v>
+      </c>
+      <c r="R99" s="3">
+        <f t="shared" si="2"/>
+        <v>1908</v>
+      </c>
+      <c r="S99" s="3">
+        <f t="shared" si="3"/>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update external growth factor.
</commit_message>
<xml_diff>
--- a/Input/controlTotals/FLUAM_DRI.xlsx
+++ b/Input/controlTotals/FLUAM_DRI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Models\StateWide\TSM_Legacy\FLUAM\Input\controlTotals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E647C-67B2-4528-920F-1BBBF97F358B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309D592B-B437-49F0-859F-CEE9395B9419}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0A4793C3-9AA2-4A53-B6D8-945A8B7F0D49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4793C3-9AA2-4A53-B6D8-945A8B7F0D49}"/>
   </bookViews>
   <sheets>
     <sheet name="DRIs" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DRI_Increment!$W$1:$Z$6425</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DRIs!$A$1:$Q$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -436,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -511,6 +512,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -826,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44179D55-CFD5-47AC-81DE-5AB054DCBB5F}">
-  <dimension ref="A1:Q99"/>
+  <dimension ref="A1:Q103"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S1" sqref="R1:S1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q103" sqref="A1:Q103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5557,272 +5559,484 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>4957</v>
-      </c>
-      <c r="B95" s="7">
-        <v>2968</v>
-      </c>
-      <c r="C95" s="7">
-        <v>1115</v>
+        <v>4860</v>
+      </c>
+      <c r="B95" s="32">
+        <v>671</v>
+      </c>
+      <c r="C95" s="32">
+        <v>839</v>
       </c>
       <c r="D95" s="9">
-        <v>3039</v>
+        <v>1366</v>
       </c>
       <c r="E95" s="9">
-        <v>1161</v>
+        <v>1291</v>
       </c>
       <c r="F95" s="9">
-        <v>3144</v>
+        <v>2061</v>
       </c>
       <c r="G95" s="9">
-        <v>1231</v>
+        <v>1743</v>
       </c>
       <c r="H95" s="9">
-        <v>3250</v>
+        <v>2756</v>
       </c>
       <c r="I95" s="9">
-        <v>1300</v>
+        <v>2195</v>
       </c>
       <c r="J95" s="9">
-        <v>3330</v>
+        <v>3451</v>
       </c>
       <c r="K95" s="9">
-        <v>1640</v>
+        <v>2647</v>
       </c>
       <c r="L95" s="9">
-        <v>3410</v>
+        <v>4146</v>
       </c>
       <c r="M95" s="9">
-        <v>1980</v>
+        <v>3099</v>
       </c>
       <c r="N95" s="9">
-        <v>3530</v>
+        <v>4841</v>
       </c>
       <c r="O95" s="9">
-        <v>2490</v>
+        <v>3551</v>
       </c>
       <c r="P95" s="8">
-        <v>3650</v>
+        <v>5535</v>
       </c>
       <c r="Q95" s="8">
-        <v>3000</v>
+        <v>4006</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>5280</v>
-      </c>
-      <c r="B96" s="7">
-        <v>905</v>
-      </c>
-      <c r="C96" s="7">
-        <v>586</v>
+        <v>4861</v>
+      </c>
+      <c r="B96" s="32">
+        <v>3293</v>
+      </c>
+      <c r="C96" s="32">
+        <v>714</v>
       </c>
       <c r="D96" s="9">
-        <v>1179</v>
+        <v>3787</v>
       </c>
       <c r="E96" s="9">
-        <v>608</v>
+        <v>2005</v>
       </c>
       <c r="F96" s="9">
-        <v>1589</v>
+        <v>4281</v>
       </c>
       <c r="G96" s="9">
-        <v>642</v>
+        <v>3296</v>
       </c>
       <c r="H96" s="9">
-        <v>2000</v>
+        <v>4775</v>
       </c>
       <c r="I96" s="9">
-        <v>675</v>
+        <v>4587</v>
       </c>
       <c r="J96" s="9">
-        <v>2650</v>
+        <v>5269</v>
       </c>
       <c r="K96" s="9">
-        <v>835</v>
+        <v>5878</v>
       </c>
       <c r="L96" s="9">
-        <v>3300</v>
+        <v>5763</v>
       </c>
       <c r="M96" s="9">
-        <v>995</v>
+        <v>7169</v>
       </c>
       <c r="N96" s="9">
-        <v>4275</v>
+        <v>6257</v>
       </c>
       <c r="O96" s="9">
-        <v>1235</v>
+        <v>8460</v>
       </c>
       <c r="P96" s="8">
-        <v>5250</v>
+        <v>6754</v>
       </c>
       <c r="Q96" s="8">
-        <v>1475</v>
+        <v>9752</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>5283</v>
-      </c>
-      <c r="B97" s="7">
-        <v>4457</v>
-      </c>
-      <c r="C97" s="7">
-        <v>2559</v>
+        <v>4902</v>
+      </c>
+      <c r="B97" s="32">
+        <v>394</v>
+      </c>
+      <c r="C97" s="32">
+        <v>1525</v>
       </c>
       <c r="D97" s="9">
-        <v>4505</v>
+        <v>667</v>
       </c>
       <c r="E97" s="9">
-        <v>2607</v>
+        <v>1632</v>
       </c>
       <c r="F97" s="9">
-        <v>4578</v>
+        <v>940</v>
       </c>
       <c r="G97" s="9">
-        <v>2678</v>
+        <v>1739</v>
       </c>
       <c r="H97" s="9">
-        <v>4650</v>
+        <v>1213</v>
       </c>
       <c r="I97" s="9">
-        <v>2750</v>
+        <v>1846</v>
       </c>
       <c r="J97" s="9">
-        <v>4720</v>
+        <v>1486</v>
       </c>
       <c r="K97" s="9">
-        <v>2800</v>
+        <v>1953</v>
       </c>
       <c r="L97" s="9">
-        <v>4790</v>
+        <v>1759</v>
       </c>
       <c r="M97" s="9">
-        <v>2850</v>
+        <v>2060</v>
       </c>
       <c r="N97" s="9">
-        <v>4895</v>
+        <v>2032</v>
       </c>
       <c r="O97" s="9">
-        <v>2925</v>
+        <v>2167</v>
       </c>
       <c r="P97" s="8">
-        <v>5000</v>
+        <v>2308</v>
       </c>
       <c r="Q97" s="8">
-        <v>3000</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>5289</v>
-      </c>
-      <c r="B98" s="7">
-        <v>4457</v>
-      </c>
-      <c r="C98" s="7">
-        <v>2559</v>
+        <v>4903</v>
+      </c>
+      <c r="B98" s="32">
+        <v>1305</v>
+      </c>
+      <c r="C98" s="32">
+        <v>648</v>
       </c>
       <c r="D98" s="9">
-        <v>4568</v>
+        <v>1701</v>
       </c>
       <c r="E98" s="9">
-        <v>2669</v>
+        <v>791</v>
       </c>
       <c r="F98" s="9">
-        <v>4734</v>
+        <v>2097</v>
       </c>
       <c r="G98" s="9">
-        <v>2835</v>
+        <v>934</v>
       </c>
       <c r="H98" s="9">
-        <v>4900</v>
+        <v>2493</v>
       </c>
       <c r="I98" s="9">
-        <v>3000</v>
+        <v>1077</v>
       </c>
       <c r="J98" s="9">
-        <v>4960</v>
+        <v>2889</v>
       </c>
       <c r="K98" s="9">
-        <v>3130</v>
+        <v>1220</v>
       </c>
       <c r="L98" s="9">
-        <v>5020</v>
+        <v>3285</v>
       </c>
       <c r="M98" s="9">
-        <v>3260</v>
+        <v>1363</v>
       </c>
       <c r="N98" s="9">
-        <v>5110</v>
+        <v>3681</v>
       </c>
       <c r="O98" s="9">
-        <v>3455</v>
+        <v>1506</v>
       </c>
       <c r="P98" s="8">
-        <v>5200</v>
+        <v>4080</v>
       </c>
       <c r="Q98" s="8">
-        <v>3650</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99">
+        <v>4957</v>
+      </c>
+      <c r="B99" s="7">
+        <v>2968</v>
+      </c>
+      <c r="C99" s="7">
+        <v>1115</v>
+      </c>
+      <c r="D99" s="9">
+        <v>3039</v>
+      </c>
+      <c r="E99" s="9">
+        <v>1161</v>
+      </c>
+      <c r="F99" s="9">
+        <v>3144</v>
+      </c>
+      <c r="G99" s="9">
+        <v>1231</v>
+      </c>
+      <c r="H99" s="9">
+        <v>3250</v>
+      </c>
+      <c r="I99" s="9">
+        <v>1300</v>
+      </c>
+      <c r="J99" s="9">
+        <v>3330</v>
+      </c>
+      <c r="K99" s="9">
+        <v>1640</v>
+      </c>
+      <c r="L99" s="9">
+        <v>3410</v>
+      </c>
+      <c r="M99" s="9">
+        <v>1980</v>
+      </c>
+      <c r="N99" s="9">
+        <v>3530</v>
+      </c>
+      <c r="O99" s="9">
+        <v>2490</v>
+      </c>
+      <c r="P99" s="8">
+        <v>3650</v>
+      </c>
+      <c r="Q99" s="8">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>5280</v>
+      </c>
+      <c r="B100" s="7">
+        <v>905</v>
+      </c>
+      <c r="C100" s="7">
+        <v>586</v>
+      </c>
+      <c r="D100" s="9">
+        <v>1179</v>
+      </c>
+      <c r="E100" s="9">
+        <v>608</v>
+      </c>
+      <c r="F100" s="9">
+        <v>1589</v>
+      </c>
+      <c r="G100" s="9">
+        <v>642</v>
+      </c>
+      <c r="H100" s="9">
+        <v>2000</v>
+      </c>
+      <c r="I100" s="9">
+        <v>675</v>
+      </c>
+      <c r="J100" s="9">
+        <v>2650</v>
+      </c>
+      <c r="K100" s="9">
+        <v>835</v>
+      </c>
+      <c r="L100" s="9">
+        <v>3300</v>
+      </c>
+      <c r="M100" s="9">
+        <v>995</v>
+      </c>
+      <c r="N100" s="9">
+        <v>4275</v>
+      </c>
+      <c r="O100" s="9">
+        <v>1235</v>
+      </c>
+      <c r="P100" s="8">
+        <v>5250</v>
+      </c>
+      <c r="Q100" s="8">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>5283</v>
+      </c>
+      <c r="B101" s="7">
+        <v>4457</v>
+      </c>
+      <c r="C101" s="7">
+        <v>2559</v>
+      </c>
+      <c r="D101" s="9">
+        <v>4505</v>
+      </c>
+      <c r="E101" s="9">
+        <v>2607</v>
+      </c>
+      <c r="F101" s="9">
+        <v>4578</v>
+      </c>
+      <c r="G101" s="9">
+        <v>2678</v>
+      </c>
+      <c r="H101" s="9">
+        <v>4650</v>
+      </c>
+      <c r="I101" s="9">
+        <v>2750</v>
+      </c>
+      <c r="J101" s="9">
+        <v>4720</v>
+      </c>
+      <c r="K101" s="9">
+        <v>2800</v>
+      </c>
+      <c r="L101" s="9">
+        <v>4790</v>
+      </c>
+      <c r="M101" s="9">
+        <v>2850</v>
+      </c>
+      <c r="N101" s="9">
+        <v>4895</v>
+      </c>
+      <c r="O101" s="9">
+        <v>2925</v>
+      </c>
+      <c r="P101" s="8">
+        <v>5000</v>
+      </c>
+      <c r="Q101" s="8">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>5289</v>
+      </c>
+      <c r="B102" s="7">
+        <v>4457</v>
+      </c>
+      <c r="C102" s="7">
+        <v>2559</v>
+      </c>
+      <c r="D102" s="9">
+        <v>4568</v>
+      </c>
+      <c r="E102" s="9">
+        <v>2669</v>
+      </c>
+      <c r="F102" s="9">
+        <v>4734</v>
+      </c>
+      <c r="G102" s="9">
+        <v>2835</v>
+      </c>
+      <c r="H102" s="9">
+        <v>4900</v>
+      </c>
+      <c r="I102" s="9">
+        <v>3000</v>
+      </c>
+      <c r="J102" s="9">
+        <v>4960</v>
+      </c>
+      <c r="K102" s="9">
+        <v>3130</v>
+      </c>
+      <c r="L102" s="9">
+        <v>5020</v>
+      </c>
+      <c r="M102" s="9">
+        <v>3260</v>
+      </c>
+      <c r="N102" s="9">
+        <v>5110</v>
+      </c>
+      <c r="O102" s="9">
+        <v>3455</v>
+      </c>
+      <c r="P102" s="8">
+        <v>5200</v>
+      </c>
+      <c r="Q102" s="8">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103">
         <v>5294</v>
       </c>
-      <c r="B99" s="7">
+      <c r="B103" s="7">
         <v>1097</v>
       </c>
-      <c r="C99" s="7">
+      <c r="C103" s="7">
         <v>73</v>
       </c>
-      <c r="D99" s="9">
+      <c r="D103" s="9">
         <v>1223</v>
       </c>
-      <c r="E99" s="9">
+      <c r="E103" s="9">
         <v>130</v>
       </c>
-      <c r="F99" s="9">
+      <c r="F103" s="9">
         <v>1411</v>
       </c>
-      <c r="G99" s="9">
+      <c r="G103" s="9">
         <v>215</v>
       </c>
-      <c r="H99" s="9">
+      <c r="H103" s="9">
         <v>1600</v>
       </c>
-      <c r="I99" s="9">
+      <c r="I103" s="9">
         <v>300</v>
       </c>
-      <c r="J99" s="9">
+      <c r="J103" s="9">
         <v>1881</v>
       </c>
-      <c r="K99" s="9">
+      <c r="K103" s="9">
         <v>340</v>
       </c>
-      <c r="L99" s="9">
+      <c r="L103" s="9">
         <v>2162</v>
       </c>
-      <c r="M99" s="9">
+      <c r="M103" s="9">
         <v>380</v>
       </c>
-      <c r="N99" s="9">
+      <c r="N103" s="9">
         <v>2584</v>
       </c>
-      <c r="O99" s="9">
+      <c r="O103" s="9">
         <v>440</v>
       </c>
-      <c r="P99" s="8">
+      <c r="P103" s="8">
         <v>3005</v>
       </c>
-      <c r="Q99" s="8">
+      <c r="Q103" s="8">
         <v>500</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q99">
-    <sortCondition ref="A2:A99"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q103">
+    <sortCondition ref="A2:A103"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5833,8 +6047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56B04E6-F45C-49E4-A13B-3B72B1122121}">
   <dimension ref="A1:S99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12898,67 +13112,67 @@
       </c>
       <c r="D95" s="4">
         <f>DRIs!D95-DRIs!B95</f>
-        <v>71</v>
+        <v>695</v>
       </c>
       <c r="E95" s="5">
         <f>DRIs!E95-DRIs!C95</f>
-        <v>46</v>
+        <v>452</v>
       </c>
       <c r="F95" s="4">
         <f>DRIs!F95-DRIs!D95</f>
-        <v>105</v>
+        <v>695</v>
       </c>
       <c r="G95" s="5">
         <f>DRIs!G95-DRIs!E95</f>
-        <v>70</v>
+        <v>452</v>
       </c>
       <c r="H95" s="4">
         <f>DRIs!H95-DRIs!F95</f>
-        <v>106</v>
+        <v>695</v>
       </c>
       <c r="I95" s="5">
         <f>DRIs!I95-DRIs!G95</f>
-        <v>69</v>
+        <v>452</v>
       </c>
       <c r="J95" s="4">
         <f>DRIs!J95-DRIs!H95</f>
-        <v>80</v>
+        <v>695</v>
       </c>
       <c r="K95" s="5">
         <f>DRIs!K95-DRIs!I95</f>
-        <v>340</v>
+        <v>452</v>
       </c>
       <c r="L95" s="4">
         <f>DRIs!L95-DRIs!J95</f>
-        <v>80</v>
+        <v>695</v>
       </c>
       <c r="M95" s="5">
         <f>DRIs!M95-DRIs!K95</f>
-        <v>340</v>
+        <v>452</v>
       </c>
       <c r="N95" s="4">
         <f>DRIs!N95-DRIs!L95</f>
-        <v>120</v>
+        <v>695</v>
       </c>
       <c r="O95" s="5">
         <f>DRIs!O95-DRIs!M95</f>
-        <v>510</v>
+        <v>452</v>
       </c>
       <c r="P95" s="6">
         <f>DRIs!P95-DRIs!N95</f>
-        <v>120</v>
+        <v>694</v>
       </c>
       <c r="Q95" s="5">
         <f>DRIs!Q95-DRIs!O95</f>
-        <v>510</v>
+        <v>455</v>
       </c>
       <c r="R95" s="3">
         <f t="shared" si="2"/>
-        <v>682</v>
+        <v>4864</v>
       </c>
       <c r="S95" s="3">
         <f t="shared" si="3"/>
-        <v>1885</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="96" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12973,67 +13187,67 @@
       </c>
       <c r="D96" s="4">
         <f>DRIs!D96-DRIs!B96</f>
-        <v>274</v>
+        <v>494</v>
       </c>
       <c r="E96" s="5">
         <f>DRIs!E96-DRIs!C96</f>
-        <v>22</v>
+        <v>1291</v>
       </c>
       <c r="F96" s="4">
         <f>DRIs!F96-DRIs!D96</f>
-        <v>410</v>
+        <v>494</v>
       </c>
       <c r="G96" s="5">
         <f>DRIs!G96-DRIs!E96</f>
-        <v>34</v>
+        <v>1291</v>
       </c>
       <c r="H96" s="4">
         <f>DRIs!H96-DRIs!F96</f>
-        <v>411</v>
+        <v>494</v>
       </c>
       <c r="I96" s="5">
         <f>DRIs!I96-DRIs!G96</f>
-        <v>33</v>
+        <v>1291</v>
       </c>
       <c r="J96" s="4">
         <f>DRIs!J96-DRIs!H96</f>
-        <v>650</v>
+        <v>494</v>
       </c>
       <c r="K96" s="5">
         <f>DRIs!K96-DRIs!I96</f>
-        <v>160</v>
+        <v>1291</v>
       </c>
       <c r="L96" s="4">
         <f>DRIs!L96-DRIs!J96</f>
-        <v>650</v>
+        <v>494</v>
       </c>
       <c r="M96" s="5">
         <f>DRIs!M96-DRIs!K96</f>
-        <v>160</v>
+        <v>1291</v>
       </c>
       <c r="N96" s="4">
         <f>DRIs!N96-DRIs!L96</f>
-        <v>975</v>
+        <v>494</v>
       </c>
       <c r="O96" s="5">
         <f>DRIs!O96-DRIs!M96</f>
-        <v>240</v>
+        <v>1291</v>
       </c>
       <c r="P96" s="6">
         <f>DRIs!P96-DRIs!N96</f>
-        <v>975</v>
+        <v>497</v>
       </c>
       <c r="Q96" s="5">
         <f>DRIs!Q96-DRIs!O96</f>
-        <v>240</v>
+        <v>1292</v>
       </c>
       <c r="R96" s="3">
         <f t="shared" si="2"/>
-        <v>4345</v>
+        <v>3461</v>
       </c>
       <c r="S96" s="3">
         <f t="shared" si="3"/>
-        <v>889</v>
+        <v>9038</v>
       </c>
     </row>
     <row r="97" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13048,67 +13262,67 @@
       </c>
       <c r="D97" s="4">
         <f>DRIs!D97-DRIs!B97</f>
-        <v>48</v>
+        <v>273</v>
       </c>
       <c r="E97" s="5">
         <f>DRIs!E97-DRIs!C97</f>
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="F97" s="4">
         <f>DRIs!F97-DRIs!D97</f>
-        <v>73</v>
+        <v>273</v>
       </c>
       <c r="G97" s="5">
         <f>DRIs!G97-DRIs!E97</f>
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="H97" s="4">
         <f>DRIs!H97-DRIs!F97</f>
-        <v>72</v>
+        <v>273</v>
       </c>
       <c r="I97" s="5">
         <f>DRIs!I97-DRIs!G97</f>
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="J97" s="4">
         <f>DRIs!J97-DRIs!H97</f>
-        <v>70</v>
+        <v>273</v>
       </c>
       <c r="K97" s="5">
         <f>DRIs!K97-DRIs!I97</f>
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="L97" s="4">
         <f>DRIs!L97-DRIs!J97</f>
-        <v>70</v>
+        <v>273</v>
       </c>
       <c r="M97" s="5">
         <f>DRIs!M97-DRIs!K97</f>
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="N97" s="4">
         <f>DRIs!N97-DRIs!L97</f>
-        <v>105</v>
+        <v>273</v>
       </c>
       <c r="O97" s="5">
         <f>DRIs!O97-DRIs!M97</f>
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="P97" s="6">
         <f>DRIs!P97-DRIs!N97</f>
-        <v>105</v>
+        <v>276</v>
       </c>
       <c r="Q97" s="5">
         <f>DRIs!Q97-DRIs!O97</f>
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="R97" s="3">
         <f t="shared" si="2"/>
-        <v>543</v>
+        <v>1914</v>
       </c>
       <c r="S97" s="3">
         <f t="shared" si="3"/>
-        <v>441</v>
+        <v>751</v>
       </c>
     </row>
     <row r="98" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13123,67 +13337,67 @@
       </c>
       <c r="D98" s="4">
         <f>DRIs!D98-DRIs!B98</f>
-        <v>111</v>
+        <v>396</v>
       </c>
       <c r="E98" s="5">
         <f>DRIs!E98-DRIs!C98</f>
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="F98" s="4">
         <f>DRIs!F98-DRIs!D98</f>
-        <v>166</v>
+        <v>396</v>
       </c>
       <c r="G98" s="5">
         <f>DRIs!G98-DRIs!E98</f>
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="H98" s="4">
         <f>DRIs!H98-DRIs!F98</f>
-        <v>166</v>
+        <v>396</v>
       </c>
       <c r="I98" s="5">
         <f>DRIs!I98-DRIs!G98</f>
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="J98" s="4">
         <f>DRIs!J98-DRIs!H98</f>
-        <v>60</v>
+        <v>396</v>
       </c>
       <c r="K98" s="5">
         <f>DRIs!K98-DRIs!I98</f>
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="L98" s="4">
         <f>DRIs!L98-DRIs!J98</f>
-        <v>60</v>
+        <v>396</v>
       </c>
       <c r="M98" s="5">
         <f>DRIs!M98-DRIs!K98</f>
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="N98" s="4">
         <f>DRIs!N98-DRIs!L98</f>
-        <v>90</v>
+        <v>396</v>
       </c>
       <c r="O98" s="5">
         <f>DRIs!O98-DRIs!M98</f>
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="P98" s="6">
         <f>DRIs!P98-DRIs!N98</f>
-        <v>90</v>
+        <v>399</v>
       </c>
       <c r="Q98" s="5">
         <f>DRIs!Q98-DRIs!O98</f>
-        <v>195</v>
+        <v>140</v>
       </c>
       <c r="R98" s="3">
         <f t="shared" si="2"/>
-        <v>743</v>
+        <v>2775</v>
       </c>
       <c r="S98" s="3">
         <f t="shared" si="3"/>
-        <v>1091</v>
+        <v>998</v>
       </c>
     </row>
     <row r="99" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13198,67 +13412,67 @@
       </c>
       <c r="D99" s="19">
         <f>DRIs!D99-DRIs!B99</f>
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="E99" s="20">
         <f>DRIs!E99-DRIs!C99</f>
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F99" s="19">
         <f>DRIs!F99-DRIs!D99</f>
-        <v>188</v>
+        <v>105</v>
       </c>
       <c r="G99" s="20">
         <f>DRIs!G99-DRIs!E99</f>
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="H99" s="19">
         <f>DRIs!H99-DRIs!F99</f>
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="I99" s="20">
         <f>DRIs!I99-DRIs!G99</f>
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="J99" s="19">
         <f>DRIs!J99-DRIs!H99</f>
-        <v>281</v>
+        <v>80</v>
       </c>
       <c r="K99" s="20">
         <f>DRIs!K99-DRIs!I99</f>
-        <v>40</v>
+        <v>340</v>
       </c>
       <c r="L99" s="19">
         <f>DRIs!L99-DRIs!J99</f>
-        <v>281</v>
+        <v>80</v>
       </c>
       <c r="M99" s="20">
         <f>DRIs!M99-DRIs!K99</f>
-        <v>40</v>
+        <v>340</v>
       </c>
       <c r="N99" s="19">
         <f>DRIs!N99-DRIs!L99</f>
-        <v>422</v>
+        <v>120</v>
       </c>
       <c r="O99" s="20">
         <f>DRIs!O99-DRIs!M99</f>
-        <v>60</v>
+        <v>510</v>
       </c>
       <c r="P99" s="21">
         <f>DRIs!P99-DRIs!N99</f>
-        <v>421</v>
+        <v>120</v>
       </c>
       <c r="Q99" s="20">
         <f>DRIs!Q99-DRIs!O99</f>
-        <v>60</v>
+        <v>510</v>
       </c>
       <c r="R99" s="3">
         <f t="shared" si="2"/>
-        <v>1908</v>
+        <v>682</v>
       </c>
       <c r="S99" s="3">
         <f t="shared" si="3"/>
-        <v>427</v>
+        <v>1885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>